<commit_message>
addded new code and frame work
</commit_message>
<xml_diff>
--- a/AutomationProject/ExcelFile/DataExcelFile.xlsx
+++ b/AutomationProject/ExcelFile/DataExcelFile.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pradeep.chauhan\eclipse-workspace2\AutomationProject\ExcelFile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="3010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,24 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Capital</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Population</t>
   </si>
   <si>
     <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>OTP</t>
   </si>
 </sst>
 </file>
@@ -362,7 +352,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -374,24 +364,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>510000017</v>
+      </c>
+      <c r="B2">
+        <v>1212</v>
       </c>
       <c r="C2">
         <v>1000</v>

</xml_diff>